<commit_message>
dosya ile masraf ekleme yapıldı. satış rakamları getirildi
</commit_message>
<xml_diff>
--- a/ActionForce/ActionForce.Office/Document/Expense/ExpenseTemplate.xlsx
+++ b/ActionForce/ActionForce.Office/Document/Expense/ExpenseTemplate.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <x:si>
     <x:t>MasrafMerkezi</x:t>
   </x:si>
@@ -119,9 +119,6 @@
     <x:t xml:space="preserve">5170 Akbatı  Trampoline  </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">5191 67 Burda Animal </x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">5210 Pomelon  Mall Moto </x:t>
   </x:si>
   <x:si>
@@ -329,7 +326,7 @@
     <x:t>Reklam, Tanıtım</x:t>
   </x:si>
   <x:si>
-    <x:t>Araç Kiralama</x:t>
+    <x:t>Araç Kiralama / Nakliye</x:t>
   </x:si>
   <x:si>
     <x:t>Sağlık</x:t>
@@ -1021,21 +1018,21 @@
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="n">
-        <x:v>106</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
         <x:v>15</x:v>
@@ -1043,10 +1040,10 @@
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="n">
-        <x:v>122</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
         <x:v>15</x:v>
@@ -1054,35 +1051,35 @@
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="n">
-        <x:v>146</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="n">
-        <x:v>126</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="n">
-        <x:v>160</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
@@ -1090,10 +1087,10 @@
         <x:v>130</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
@@ -1101,7 +1098,7 @@
         <x:v>134</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
         <x:v>17</x:v>
@@ -1112,7 +1109,7 @@
         <x:v>135</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
         <x:v>15</x:v>
@@ -1123,10 +1120,10 @@
         <x:v>226</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
@@ -1134,7 +1131,7 @@
         <x:v>141</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
         <x:v>15</x:v>
@@ -1145,7 +1142,7 @@
         <x:v>149</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
         <x:v>15</x:v>
@@ -1156,7 +1153,7 @@
         <x:v>167</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
         <x:v>17</x:v>
@@ -1167,7 +1164,7 @@
         <x:v>163</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
         <x:v>15</x:v>
@@ -1178,7 +1175,7 @@
         <x:v>165</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>17</x:v>
@@ -1189,7 +1186,7 @@
         <x:v>168</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
         <x:v>15</x:v>
@@ -1200,7 +1197,7 @@
         <x:v>169</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
         <x:v>15</x:v>
@@ -1211,7 +1208,7 @@
         <x:v>171</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
         <x:v>15</x:v>
@@ -1222,7 +1219,7 @@
         <x:v>176</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
         <x:v>15</x:v>
@@ -1233,7 +1230,7 @@
         <x:v>177</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
         <x:v>17</x:v>
@@ -1244,7 +1241,7 @@
         <x:v>183</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
         <x:v>15</x:v>
@@ -1255,10 +1252,10 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
@@ -1266,7 +1263,7 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
         <x:v>15</x:v>
@@ -1277,7 +1274,7 @@
         <x:v>211</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
         <x:v>17</x:v>
@@ -1288,10 +1285,10 @@
         <x:v>213</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3">
@@ -1299,7 +1296,7 @@
         <x:v>193</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
         <x:v>17</x:v>
@@ -1310,7 +1307,7 @@
         <x:v>196</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
         <x:v>17</x:v>
@@ -1321,7 +1318,7 @@
         <x:v>199</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
         <x:v>17</x:v>
@@ -1332,7 +1329,7 @@
         <x:v>200</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
         <x:v>15</x:v>
@@ -1343,7 +1340,7 @@
         <x:v>201</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
         <x:v>15</x:v>
@@ -1354,7 +1351,7 @@
         <x:v>202</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
         <x:v>15</x:v>
@@ -1365,7 +1362,7 @@
         <x:v>214</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
         <x:v>17</x:v>
@@ -1376,10 +1373,10 @@
         <x:v>218</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3">
@@ -1387,7 +1384,7 @@
         <x:v>219</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
         <x:v>15</x:v>
@@ -1398,10 +1395,10 @@
         <x:v>220</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:3">
@@ -1409,10 +1406,10 @@
         <x:v>221</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:3">
@@ -1420,7 +1417,7 @@
         <x:v>222</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
         <x:v>19</x:v>
@@ -1431,7 +1428,7 @@
         <x:v>224</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
         <x:v>15</x:v>
@@ -1442,10 +1439,10 @@
         <x:v>225</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:3">
@@ -1453,7 +1450,7 @@
         <x:v>228</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
         <x:v>19</x:v>
@@ -1464,10 +1461,10 @@
         <x:v>227</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
         <x:v>69</x:v>
-      </x:c>
-      <x:c r="C56" s="0" t="s">
-        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:3">
@@ -1475,10 +1472,10 @@
         <x:v>229</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:3">
@@ -1486,7 +1483,7 @@
         <x:v>230</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
         <x:v>19</x:v>
@@ -1497,7 +1494,7 @@
         <x:v>231</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
         <x:v>17</x:v>
@@ -1508,7 +1505,7 @@
         <x:v>232</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
         <x:v>19</x:v>
@@ -1519,7 +1516,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
         <x:v>17</x:v>
@@ -1530,7 +1527,7 @@
         <x:v>234</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
         <x:v>15</x:v>
@@ -1541,7 +1538,7 @@
         <x:v>235</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
         <x:v>17</x:v>
@@ -1572,7 +1569,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
@@ -1580,7 +1577,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1588,7 +1585,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1596,7 +1593,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1624,7 +1621,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
@@ -1632,7 +1629,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1640,7 +1637,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>83</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1648,7 +1645,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1656,7 +1653,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1664,7 +1661,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1672,7 +1669,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1680,7 +1677,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1688,7 +1685,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1696,7 +1693,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1704,7 +1701,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1712,7 +1709,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1720,7 +1717,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1728,7 +1725,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1736,7 +1733,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1744,7 +1741,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1752,7 +1749,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1760,7 +1757,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1768,7 +1765,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1776,7 +1773,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>100</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1784,7 +1781,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:2">
@@ -1792,7 +1789,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:2">
@@ -1800,7 +1797,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:2">
@@ -1808,7 +1805,7 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:2">
@@ -1816,7 +1813,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:2">
@@ -1824,7 +1821,7 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:2">
@@ -1832,7 +1829,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:2">
@@ -1840,7 +1837,7 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:2">
@@ -1848,7 +1845,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:2">
@@ -1856,7 +1853,7 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:2">
@@ -1864,7 +1861,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:2">
@@ -1872,7 +1869,7 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:2">
@@ -1880,7 +1877,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:2">
@@ -1888,7 +1885,7 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:2">
@@ -1896,7 +1893,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:2">
@@ -1904,7 +1901,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:2">
@@ -1912,7 +1909,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:2">
@@ -1920,7 +1917,7 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:2">
@@ -1928,7 +1925,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:2">
@@ -1936,7 +1933,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:2">
@@ -1944,7 +1941,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>121</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:2">
@@ -1952,7 +1949,7 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:2">
@@ -1960,7 +1957,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:2">
@@ -1968,7 +1965,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:2">
@@ -1976,7 +1973,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:2">
@@ -1984,7 +1981,7 @@
         <x:v>45</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:2">
@@ -1992,7 +1989,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:2">
@@ -2000,7 +1997,7 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2028,10 +2025,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
         <x:v>129</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
@@ -2042,7 +2039,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
@@ -2050,10 +2047,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>132</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>133</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -2061,10 +2058,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>134</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>135</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
@@ -2072,10 +2069,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>136</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
@@ -2083,10 +2080,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>138</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>139</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>